<commit_message>
db, json, wd utility
</commit_message>
<xml_diff>
--- a/ninjacrm-automation-framework/src/test/resources/testData.xlsx
+++ b/ninjacrm-automation-framework/src/test/resources/testData.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Basic_Selenium\ninjacrm-automation-framework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\NinjaCRM-FW\ninjacrm-automation-framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Opp" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Opportunity ID</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Priya Sharma</t>
   </si>
   <si>
-    <t>2025-09-04</t>
-  </si>
-  <si>
     <t>2025-10-05</t>
   </si>
   <si>
@@ -214,6 +211,15 @@
   </si>
   <si>
     <t>This is a potential deal for E-Commerce Website Revamp project.</t>
+  </si>
+  <si>
+    <t>26847</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>04-06-2025</t>
   </si>
 </sst>
 </file>
@@ -278,12 +284,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +599,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,8 +658,8 @@
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1">
-        <v>26847</v>
+      <c r="C2" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
@@ -659,23 +667,23 @@
       <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
+      <c r="F2" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="1">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -695,22 +703,22 @@
         <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="1">
         <v>63</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -730,22 +738,22 @@
         <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="1">
         <v>82</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -765,22 +773,22 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" s="1">
         <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,22 +808,22 @@
         <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1">
         <v>38</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -835,22 +843,22 @@
         <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" s="1">
         <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -870,22 +878,22 @@
         <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1">
         <v>76</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -905,22 +913,22 @@
         <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="1">
         <v>77</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -940,22 +948,22 @@
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="1">
         <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -975,22 +983,22 @@
         <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" s="1">
         <v>99</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>